<commit_message>
added July review options
</commit_message>
<xml_diff>
--- a/doc/figs/calendar.xlsx
+++ b/doc/figs/calendar.xlsx
@@ -106,7 +106,7 @@
   <numFmts count="3">
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="173" formatCode="d"/>
+    <numFmt numFmtId="164" formatCode="d"/>
   </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
@@ -396,7 +396,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="33">
+  <borders count="31">
     <border>
       <left/>
       <right/>
@@ -432,24 +432,6 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -3141,15 +3123,15 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="173" fontId="16" fillId="22" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="16" fillId="22" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="173" fontId="16" fillId="22" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="16" fillId="22" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="173" fontId="16" fillId="22" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="16" fillId="22" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -3187,129 +3169,129 @@
     <xf numFmtId="0" fontId="11" fillId="23" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="5" xfId="2302" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="3" xfId="2302" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="6" xfId="2302" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="4" xfId="2302" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="7" xfId="2302" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="5" xfId="2302" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="9" xfId="2302" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="7" xfId="2302" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="173" fontId="16" fillId="26" borderId="10" xfId="1838" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="16" fillId="26" borderId="8" xfId="1838" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="173" fontId="16" fillId="22" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="16" fillId="22" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="173" fontId="16" fillId="26" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="16" fillId="26" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="173" fontId="16" fillId="22" borderId="11" xfId="1838" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="16" fillId="22" borderId="9" xfId="1838" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="173" fontId="16" fillId="26" borderId="12" xfId="1838" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="16" fillId="26" borderId="10" xfId="1838" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="173" fontId="16" fillId="17" borderId="12" xfId="1838" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="16" fillId="17" borderId="10" xfId="1838" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="173" fontId="16" fillId="22" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="16" fillId="22" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="173" fontId="16" fillId="26" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="16" fillId="26" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="173" fontId="16" fillId="22" borderId="14" xfId="1838" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="16" fillId="22" borderId="12" xfId="1838" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="173" fontId="17" fillId="25" borderId="15" xfId="1838" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="17" fillId="25" borderId="13" xfId="1838" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="173" fontId="16" fillId="26" borderId="15" xfId="1838" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="16" fillId="26" borderId="13" xfId="1838" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="173" fontId="16" fillId="17" borderId="14" xfId="1838" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="16" fillId="17" borderId="12" xfId="1838" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="173" fontId="16" fillId="17" borderId="15" xfId="1838" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="16" fillId="17" borderId="13" xfId="1838" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="173" fontId="17" fillId="25" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="17" fillId="25" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="173" fontId="16" fillId="22" borderId="17" xfId="1838" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="16" fillId="22" borderId="15" xfId="1838" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="173" fontId="16" fillId="26" borderId="18" xfId="1838" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="16" fillId="26" borderId="16" xfId="1838" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="173" fontId="16" fillId="22" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="16" fillId="22" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="173" fontId="16" fillId="26" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="16" fillId="26" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="173" fontId="16" fillId="22" borderId="20" xfId="1838" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="16" fillId="22" borderId="18" xfId="1838" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="19" xfId="2302" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="20" xfId="2302" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="24" borderId="21" xfId="2302" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="22" xfId="2302" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="16" fillId="22" borderId="22" xfId="1838" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="26" borderId="23" xfId="1838" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="26" borderId="24" xfId="1838" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="25" xfId="2302" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="23" xfId="2302" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="173" fontId="16" fillId="22" borderId="24" xfId="1838" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="173" fontId="16" fillId="26" borderId="25" xfId="1838" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="173" fontId="16" fillId="26" borderId="26" xfId="1838" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="27" xfId="2302" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="173" fontId="16" fillId="22" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="16" fillId="22" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1838" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="173" fontId="16" fillId="22" borderId="29" xfId="1838" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="16" fillId="22" borderId="27" xfId="1838" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="173" fontId="17" fillId="22" borderId="11" xfId="1838" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="17" fillId="22" borderId="9" xfId="1838" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="173" fontId="16" fillId="27" borderId="12" xfId="1838" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="16" fillId="27" borderId="10" xfId="1838" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="173" fontId="16" fillId="28" borderId="15" xfId="1838" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="16" fillId="28" borderId="13" xfId="1838" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="173" fontId="16" fillId="28" borderId="18" xfId="1838" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="16" fillId="28" borderId="16" xfId="1838" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="173" fontId="17" fillId="25" borderId="26" xfId="1838" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="17" fillId="25" borderId="24" xfId="1838" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="30" xfId="2302" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="28" xfId="2302" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="10" fillId="21" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="173" fontId="17" fillId="25" borderId="12" xfId="1838" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="17" fillId="25" borderId="10" xfId="1838" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="173" fontId="17" fillId="25" borderId="18" xfId="1838" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="17" fillId="25" borderId="16" xfId="1838" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="28" borderId="0" xfId="1838" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3318,64 +3300,52 @@
     <xf numFmtId="0" fontId="16" fillId="28" borderId="0" xfId="1838" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="173" fontId="16" fillId="15" borderId="10" xfId="1838" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="16" fillId="15" borderId="8" xfId="1838" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="173" fontId="16" fillId="22" borderId="8" xfId="1838" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="16" fillId="22" borderId="6" xfId="1838" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="173" fontId="16" fillId="22" borderId="13" xfId="1838" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="16" fillId="22" borderId="11" xfId="1838" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="173" fontId="16" fillId="22" borderId="16" xfId="1838" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="16" fillId="22" borderId="14" xfId="1838" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="173" fontId="16" fillId="22" borderId="19" xfId="1838" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="16" fillId="22" borderId="17" xfId="1838" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="173" fontId="16" fillId="22" borderId="31" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="16" fillId="22" borderId="29" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="32" xfId="2302" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="30" xfId="2302" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="173" fontId="16" fillId="26" borderId="0" xfId="1838" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="16" fillId="22" borderId="26" xfId="1838" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="173" fontId="16" fillId="22" borderId="3" xfId="1838" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="11" fillId="22" borderId="17" xfId="1838" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="173" fontId="16" fillId="22" borderId="4" xfId="1838" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="173" fontId="16" fillId="22" borderId="28" xfId="1838" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="173" fontId="11" fillId="22" borderId="19" xfId="1838" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="173" fontId="11" fillId="0" borderId="15" xfId="1838" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="13" xfId="1838" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="173" fontId="16" fillId="0" borderId="10" xfId="1838" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="8" xfId="1838" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="173" fontId="16" fillId="0" borderId="12" xfId="1838" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="10" xfId="1838" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="173" fontId="16" fillId="0" borderId="15" xfId="1838" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="13" xfId="1838" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="173" fontId="16" fillId="0" borderId="18" xfId="1838" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="16" xfId="1838" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="173" fontId="16" fillId="0" borderId="25" xfId="1838" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="173" fontId="16" fillId="0" borderId="0" xfId="1838" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="23" xfId="1838" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -3396,6 +3366,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="19" borderId="13" xfId="1838" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2304">
@@ -5708,6 +5681,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFD2E0B2"/>
       <color rgb="FFFFD1E8"/>
       <color rgb="FFF7CD89"/>
     </mruColors>
@@ -5988,8 +5962,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:AF35"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="B34" sqref="B1:AF34"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="V32" sqref="V32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6166,13 +6140,13 @@
       <c r="R4" s="26"/>
       <c r="S4" s="25"/>
       <c r="T4" s="25"/>
-      <c r="U4" s="81">
+      <c r="U4" s="78">
         <v>1</v>
       </c>
-      <c r="V4" s="82">
+      <c r="V4" s="79">
         <v>2</v>
       </c>
-      <c r="W4" s="82">
+      <c r="W4" s="79">
         <v>3</v>
       </c>
       <c r="X4" s="69">
@@ -6237,13 +6211,13 @@
       <c r="R5" s="35">
         <v>5</v>
       </c>
-      <c r="S5" s="83">
+      <c r="S5" s="80">
         <v>6</v>
       </c>
-      <c r="T5" s="83">
+      <c r="T5" s="80">
         <v>7</v>
       </c>
-      <c r="U5" s="83">
+      <c r="U5" s="80">
         <v>8</v>
       </c>
       <c r="V5" s="31">
@@ -6262,16 +6236,16 @@
       <c r="AA5" s="31">
         <v>3</v>
       </c>
-      <c r="AB5" s="83">
+      <c r="AB5" s="80">
         <v>4</v>
       </c>
-      <c r="AC5" s="83">
+      <c r="AC5" s="80">
         <v>5</v>
       </c>
-      <c r="AD5" s="83">
+      <c r="AD5" s="80">
         <v>6</v>
       </c>
-      <c r="AE5" s="83">
+      <c r="AE5" s="80">
         <v>7</v>
       </c>
       <c r="AF5" s="70">
@@ -6304,7 +6278,7 @@
       <c r="J6" s="35">
         <v>12</v>
       </c>
-      <c r="K6" s="80">
+      <c r="K6" s="77">
         <v>13</v>
       </c>
       <c r="L6" s="37">
@@ -6348,10 +6322,10 @@
       <c r="Z6" s="41">
         <v>9</v>
       </c>
-      <c r="AA6" s="84">
+      <c r="AA6" s="81">
         <v>10</v>
       </c>
-      <c r="AB6" s="84">
+      <c r="AB6" s="81">
         <v>11</v>
       </c>
       <c r="AC6" s="37">
@@ -6437,22 +6411,22 @@
       <c r="Z7" s="41">
         <v>16</v>
       </c>
-      <c r="AA7" s="42">
+      <c r="AA7" s="81">
         <v>17</v>
       </c>
-      <c r="AB7" s="42">
+      <c r="AB7" s="81">
         <v>18</v>
       </c>
-      <c r="AC7" s="42">
+      <c r="AC7" s="37">
         <v>19</v>
       </c>
-      <c r="AD7" s="42">
+      <c r="AD7" s="37">
         <v>20</v>
       </c>
-      <c r="AE7" s="42">
+      <c r="AE7" s="37">
         <v>21</v>
       </c>
-      <c r="AF7" s="72">
+      <c r="AF7" s="71">
         <v>22</v>
       </c>
     </row>
@@ -6505,25 +6479,25 @@
       </c>
       <c r="X8" s="48"/>
       <c r="Y8" s="4"/>
-      <c r="Z8" s="76">
+      <c r="Z8" s="41">
         <v>23</v>
       </c>
-      <c r="AA8" s="75">
+      <c r="AA8" s="81">
         <v>24</v>
       </c>
-      <c r="AB8" s="75">
+      <c r="AB8" s="81">
         <v>25</v>
       </c>
-      <c r="AC8" s="75">
+      <c r="AC8" s="37">
         <v>26</v>
       </c>
-      <c r="AD8" s="75">
+      <c r="AD8" s="37">
         <v>27</v>
       </c>
-      <c r="AE8" s="75">
+      <c r="AE8" s="37">
         <v>28</v>
       </c>
-      <c r="AF8" s="77">
+      <c r="AF8" s="71">
         <v>29</v>
       </c>
     </row>
@@ -6735,7 +6709,7 @@
       <c r="G13" s="29">
         <v>5</v>
       </c>
-      <c r="H13" s="78">
+      <c r="H13" s="75">
         <v>6</v>
       </c>
       <c r="I13" s="4"/>
@@ -6785,19 +6759,19 @@
       <c r="B14" s="30">
         <v>7</v>
       </c>
-      <c r="C14" s="83">
+      <c r="C14" s="80">
         <v>8</v>
       </c>
-      <c r="D14" s="83">
+      <c r="D14" s="80">
         <v>9</v>
       </c>
-      <c r="E14" s="83">
+      <c r="E14" s="80">
         <v>10</v>
       </c>
-      <c r="F14" s="83">
+      <c r="F14" s="80">
         <v>11</v>
       </c>
-      <c r="G14" s="83">
+      <c r="G14" s="80">
         <v>12</v>
       </c>
       <c r="H14" s="70">
@@ -6807,19 +6781,19 @@
       <c r="J14" s="30">
         <v>4</v>
       </c>
-      <c r="K14" s="83">
+      <c r="K14" s="80">
         <v>5</v>
       </c>
-      <c r="L14" s="83">
+      <c r="L14" s="80">
         <v>6</v>
       </c>
-      <c r="M14" s="83">
+      <c r="M14" s="80">
         <v>7</v>
       </c>
-      <c r="N14" s="83">
+      <c r="N14" s="80">
         <v>8</v>
       </c>
-      <c r="O14" s="83">
+      <c r="O14" s="80">
         <v>9</v>
       </c>
       <c r="P14" s="70">
@@ -6860,10 +6834,10 @@
       <c r="AC14" s="31">
         <v>9</v>
       </c>
-      <c r="AD14" s="31">
+      <c r="AD14" s="58">
         <v>10</v>
       </c>
-      <c r="AE14" s="58">
+      <c r="AE14" s="31">
         <v>11</v>
       </c>
       <c r="AF14" s="70">
@@ -6874,19 +6848,19 @@
       <c r="B15" s="35">
         <v>14</v>
       </c>
-      <c r="C15" s="84">
+      <c r="C15" s="81">
         <v>15</v>
       </c>
-      <c r="D15" s="84">
+      <c r="D15" s="81">
         <v>16</v>
       </c>
-      <c r="E15" s="84">
+      <c r="E15" s="81">
         <v>17</v>
       </c>
-      <c r="F15" s="84">
+      <c r="F15" s="81">
         <v>18</v>
       </c>
-      <c r="G15" s="84">
+      <c r="G15" s="81">
         <v>19</v>
       </c>
       <c r="H15" s="71">
@@ -6918,19 +6892,19 @@
       <c r="R15" s="35">
         <v>9</v>
       </c>
-      <c r="S15" s="84">
+      <c r="S15" s="95">
         <v>10</v>
       </c>
-      <c r="T15" s="84">
+      <c r="T15" s="95">
         <v>11</v>
       </c>
-      <c r="U15" s="84">
+      <c r="U15" s="95">
         <v>12</v>
       </c>
-      <c r="V15" s="84">
+      <c r="V15" s="95">
         <v>13</v>
       </c>
-      <c r="W15" s="84">
+      <c r="W15" s="95">
         <v>14</v>
       </c>
       <c r="X15" s="71">
@@ -6963,19 +6937,19 @@
       <c r="B16" s="35">
         <v>21</v>
       </c>
-      <c r="C16" s="84">
+      <c r="C16" s="81">
         <v>22</v>
       </c>
-      <c r="D16" s="84">
+      <c r="D16" s="81">
         <v>23</v>
       </c>
-      <c r="E16" s="85">
+      <c r="E16" s="82">
         <v>24</v>
       </c>
-      <c r="F16" s="84">
+      <c r="F16" s="81">
         <v>25</v>
       </c>
-      <c r="G16" s="84">
+      <c r="G16" s="81">
         <v>26</v>
       </c>
       <c r="H16" s="71">
@@ -6988,41 +6962,41 @@
       <c r="K16" s="36">
         <v>19</v>
       </c>
-      <c r="L16" s="85">
+      <c r="L16" s="82">
         <v>20</v>
       </c>
-      <c r="M16" s="85">
+      <c r="M16" s="82">
         <v>21</v>
       </c>
-      <c r="N16" s="85">
+      <c r="N16" s="82">
         <v>22</v>
       </c>
-      <c r="O16" s="85">
+      <c r="O16" s="82">
         <v>23</v>
       </c>
       <c r="P16" s="71">
         <v>24</v>
       </c>
       <c r="Q16" s="4"/>
-      <c r="R16" s="41">
+      <c r="R16" s="35">
         <v>16</v>
       </c>
-      <c r="S16" s="85">
+      <c r="S16" s="95">
         <v>17</v>
       </c>
-      <c r="T16" s="85">
+      <c r="T16" s="95">
         <v>18</v>
       </c>
-      <c r="U16" s="85">
+      <c r="U16" s="95">
         <v>19</v>
       </c>
-      <c r="V16" s="85">
+      <c r="V16" s="95">
         <v>20</v>
       </c>
-      <c r="W16" s="85">
+      <c r="W16" s="95">
         <v>21</v>
       </c>
-      <c r="X16" s="72">
+      <c r="X16" s="71">
         <v>22</v>
       </c>
       <c r="Y16" s="4"/>
@@ -7068,10 +7042,10 @@
       <c r="J17" s="49">
         <v>25</v>
       </c>
-      <c r="K17" s="86">
+      <c r="K17" s="83">
         <v>26</v>
       </c>
-      <c r="L17" s="86">
+      <c r="L17" s="83">
         <v>27</v>
       </c>
       <c r="M17" s="51">
@@ -7085,25 +7059,25 @@
       </c>
       <c r="P17" s="48"/>
       <c r="Q17" s="4"/>
-      <c r="R17" s="76">
+      <c r="R17" s="35">
         <v>23</v>
       </c>
-      <c r="S17" s="87">
+      <c r="S17" s="95">
         <v>24</v>
       </c>
-      <c r="T17" s="87">
+      <c r="T17" s="95">
         <v>25</v>
       </c>
-      <c r="U17" s="87">
+      <c r="U17" s="95">
         <v>26</v>
       </c>
-      <c r="V17" s="87">
+      <c r="V17" s="95">
         <v>27</v>
       </c>
-      <c r="W17" s="87">
+      <c r="W17" s="95">
         <v>28</v>
       </c>
-      <c r="X17" s="77">
+      <c r="X17" s="71">
         <v>29</v>
       </c>
       <c r="Y17" s="4"/>
@@ -7391,7 +7365,7 @@
       <c r="D23" s="31">
         <v>5</v>
       </c>
-      <c r="E23" s="83">
+      <c r="E23" s="80">
         <v>6</v>
       </c>
       <c r="F23" s="32">
@@ -7518,19 +7492,19 @@
       <c r="R24" s="35">
         <v>12</v>
       </c>
-      <c r="S24" s="84">
+      <c r="S24" s="81">
         <v>13</v>
       </c>
-      <c r="T24" s="84">
+      <c r="T24" s="81">
         <v>14</v>
       </c>
-      <c r="U24" s="84">
+      <c r="U24" s="81">
         <v>15</v>
       </c>
-      <c r="V24" s="84">
+      <c r="V24" s="81">
         <v>16</v>
       </c>
-      <c r="W24" s="84">
+      <c r="W24" s="81">
         <v>17</v>
       </c>
       <c r="X24" s="71">
@@ -7607,7 +7581,7 @@
       <c r="R25" s="35">
         <v>19</v>
       </c>
-      <c r="S25" s="85">
+      <c r="S25" s="82">
         <v>20</v>
       </c>
       <c r="T25" s="42">
@@ -7644,7 +7618,7 @@
       <c r="AE25" s="42">
         <v>22</v>
       </c>
-      <c r="AF25" s="79">
+      <c r="AF25" s="76">
         <v>23</v>
       </c>
     </row>
@@ -7831,27 +7805,27 @@
       <c r="AF29" s="4"/>
     </row>
     <row r="30" spans="2:32" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="88" t="s">
+      <c r="B30" s="84" t="s">
         <v>21</v>
       </c>
-      <c r="C30" s="89"/>
-      <c r="D30" s="89"/>
-      <c r="E30" s="89"/>
-      <c r="F30" s="89"/>
-      <c r="G30" s="89"/>
-      <c r="H30" s="89"/>
-      <c r="I30" s="90"/>
-      <c r="J30" s="90"/>
-      <c r="K30" s="90"/>
-      <c r="L30" s="91"/>
-      <c r="M30" s="95"/>
-      <c r="N30" s="95"/>
-      <c r="O30" s="95"/>
-      <c r="P30" s="95"/>
-      <c r="Q30" s="95"/>
-      <c r="R30" s="96"/>
-      <c r="S30" s="96"/>
-      <c r="T30" s="96"/>
+      <c r="C30" s="85"/>
+      <c r="D30" s="85"/>
+      <c r="E30" s="85"/>
+      <c r="F30" s="85"/>
+      <c r="G30" s="85"/>
+      <c r="H30" s="85"/>
+      <c r="I30" s="86"/>
+      <c r="J30" s="86"/>
+      <c r="K30" s="86"/>
+      <c r="L30" s="87"/>
+      <c r="M30" s="91"/>
+      <c r="N30" s="91"/>
+      <c r="O30" s="91"/>
+      <c r="P30" s="91"/>
+      <c r="Q30" s="91"/>
+      <c r="R30" s="92"/>
+      <c r="S30" s="92"/>
+      <c r="T30" s="92"/>
       <c r="U30" s="4"/>
       <c r="V30" s="4"/>
       <c r="W30" s="4"/>
@@ -7875,18 +7849,18 @@
       <c r="F31" s="16"/>
       <c r="G31" s="16"/>
       <c r="H31" s="16"/>
-      <c r="I31" s="91"/>
-      <c r="J31" s="91"/>
-      <c r="K31" s="91"/>
-      <c r="L31" s="91"/>
-      <c r="M31" s="95"/>
-      <c r="N31" s="97"/>
-      <c r="O31" s="98"/>
-      <c r="P31" s="98"/>
-      <c r="Q31" s="98"/>
-      <c r="R31" s="96"/>
-      <c r="S31" s="96"/>
-      <c r="T31" s="96"/>
+      <c r="I31" s="87"/>
+      <c r="J31" s="87"/>
+      <c r="K31" s="87"/>
+      <c r="L31" s="87"/>
+      <c r="M31" s="91"/>
+      <c r="N31" s="93"/>
+      <c r="O31" s="94"/>
+      <c r="P31" s="94"/>
+      <c r="Q31" s="94"/>
+      <c r="R31" s="92"/>
+      <c r="S31" s="92"/>
+      <c r="T31" s="92"/>
       <c r="U31" s="4"/>
       <c r="V31" s="4"/>
       <c r="W31" s="4"/>
@@ -7910,18 +7884,18 @@
       <c r="F32" s="18"/>
       <c r="G32" s="18"/>
       <c r="H32" s="18"/>
-      <c r="I32" s="91"/>
-      <c r="J32" s="91"/>
-      <c r="K32" s="91"/>
-      <c r="L32" s="91"/>
-      <c r="M32" s="95"/>
-      <c r="N32" s="97"/>
-      <c r="O32" s="98"/>
-      <c r="P32" s="98"/>
-      <c r="Q32" s="98"/>
-      <c r="R32" s="96"/>
-      <c r="S32" s="96"/>
-      <c r="T32" s="96"/>
+      <c r="I32" s="87"/>
+      <c r="J32" s="87"/>
+      <c r="K32" s="87"/>
+      <c r="L32" s="87"/>
+      <c r="M32" s="91"/>
+      <c r="N32" s="93"/>
+      <c r="O32" s="94"/>
+      <c r="P32" s="94"/>
+      <c r="Q32" s="94"/>
+      <c r="R32" s="92"/>
+      <c r="S32" s="92"/>
+      <c r="T32" s="92"/>
       <c r="U32" s="4"/>
       <c r="V32" s="4"/>
       <c r="W32" s="4"/>
@@ -7937,18 +7911,18 @@
       <c r="F33" s="67"/>
       <c r="G33" s="67"/>
       <c r="H33" s="67"/>
-      <c r="I33" s="92"/>
-      <c r="J33" s="92"/>
-      <c r="K33" s="92"/>
-      <c r="L33" s="92"/>
-      <c r="M33" s="92"/>
-      <c r="N33" s="92"/>
-      <c r="O33" s="95"/>
-      <c r="P33" s="95"/>
-      <c r="Q33" s="95"/>
-      <c r="R33" s="96"/>
-      <c r="S33" s="96"/>
-      <c r="T33" s="96"/>
+      <c r="I33" s="88"/>
+      <c r="J33" s="88"/>
+      <c r="K33" s="88"/>
+      <c r="L33" s="88"/>
+      <c r="M33" s="88"/>
+      <c r="N33" s="88"/>
+      <c r="O33" s="91"/>
+      <c r="P33" s="91"/>
+      <c r="Q33" s="91"/>
+      <c r="R33" s="92"/>
+      <c r="S33" s="92"/>
+      <c r="T33" s="92"/>
       <c r="U33" s="4"/>
       <c r="V33" s="4"/>
       <c r="W33" s="4"/>
@@ -7964,15 +7938,15 @@
       <c r="F34" s="20"/>
       <c r="G34" s="20"/>
       <c r="H34" s="20"/>
-      <c r="I34" s="93"/>
-      <c r="J34" s="93"/>
-      <c r="K34" s="93"/>
-      <c r="L34" s="94"/>
-      <c r="M34" s="94"/>
-      <c r="N34" s="94"/>
-      <c r="O34" s="94"/>
-      <c r="P34" s="94"/>
-      <c r="Q34" s="94"/>
+      <c r="I34" s="89"/>
+      <c r="J34" s="89"/>
+      <c r="K34" s="89"/>
+      <c r="L34" s="90"/>
+      <c r="M34" s="90"/>
+      <c r="N34" s="90"/>
+      <c r="O34" s="90"/>
+      <c r="P34" s="90"/>
+      <c r="Q34" s="90"/>
       <c r="R34" s="4"/>
       <c r="S34" s="4"/>
       <c r="T34" s="4"/>

</xml_diff>